<commit_message>
Generic paths, knn and svm for artist classifiers ready to use; other fixes
</commit_message>
<xml_diff>
--- a/assets/predictions_artist.xlsx
+++ b/assets/predictions_artist.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2044,7 +2044,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2248,7 +2248,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2520,7 +2520,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2945,7 +2945,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3064,7 +3064,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3268,7 +3268,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3608,7 +3608,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3642,7 +3642,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3778,7 +3778,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3829,7 +3829,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3863,7 +3863,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3931,7 +3931,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4016,7 +4016,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4203,7 +4203,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4271,7 +4271,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4322,7 +4322,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4441,7 +4441,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4492,7 +4492,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4577,7 +4577,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4798,7 +4798,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4815,7 +4815,7 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4883,7 +4883,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4900,7 +4900,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4968,7 +4968,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5002,7 +5002,7 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5019,7 +5019,7 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5121,7 +5121,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5138,7 +5138,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5155,7 +5155,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5189,7 +5189,7 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5223,7 +5223,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5240,7 +5240,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5342,7 +5342,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5444,7 +5444,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -5495,7 +5495,7 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5580,7 +5580,7 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5665,7 +5665,7 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5699,7 +5699,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5750,7 +5750,7 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5784,7 +5784,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5818,7 +5818,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5869,7 +5869,7 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6073,7 +6073,7 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6124,7 +6124,7 @@
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6209,7 +6209,7 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6226,7 +6226,7 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6294,7 +6294,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6311,7 +6311,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6379,7 +6379,7 @@
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6430,7 +6430,7 @@
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6481,7 +6481,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6668,7 +6668,7 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6685,7 +6685,7 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6702,7 +6702,7 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6719,7 +6719,7 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6770,7 +6770,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6821,7 +6821,7 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6872,7 +6872,7 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6940,7 +6940,7 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6957,7 +6957,7 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7025,7 +7025,7 @@
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7110,7 +7110,7 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7314,7 +7314,7 @@
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7399,7 +7399,7 @@
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7552,7 +7552,7 @@
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7569,7 +7569,7 @@
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7586,7 +7586,7 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7637,7 +7637,7 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7688,7 +7688,7 @@
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7705,7 +7705,7 @@
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7756,7 +7756,7 @@
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7773,7 +7773,7 @@
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7807,7 +7807,7 @@
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -7824,7 +7824,7 @@
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7892,7 +7892,7 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7909,7 +7909,7 @@
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7960,7 +7960,7 @@
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8028,7 +8028,7 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8096,7 +8096,7 @@
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8147,7 +8147,7 @@
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8283,7 +8283,7 @@
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8351,7 +8351,7 @@
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8504,7 +8504,7 @@
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8572,7 +8572,7 @@
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8606,7 +8606,7 @@
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8776,7 +8776,7 @@
       </c>
       <c r="C491" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8793,7 +8793,7 @@
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8827,7 +8827,7 @@
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8844,7 +8844,7 @@
       </c>
       <c r="C495" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8878,7 +8878,7 @@
       </c>
       <c r="C497" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8980,7 +8980,7 @@
       </c>
       <c r="C503" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9014,7 +9014,7 @@
       </c>
       <c r="C505" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9218,7 +9218,7 @@
       </c>
       <c r="C517" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9269,7 +9269,7 @@
       </c>
       <c r="C520" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9286,7 +9286,7 @@
       </c>
       <c r="C521" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9320,7 +9320,7 @@
       </c>
       <c r="C523" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -9337,7 +9337,7 @@
       </c>
       <c r="C524" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9388,7 +9388,7 @@
       </c>
       <c r="C527" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9541,7 +9541,7 @@
       </c>
       <c r="C536" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9745,7 +9745,7 @@
       </c>
       <c r="C548" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9796,7 +9796,7 @@
       </c>
       <c r="C551" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9813,7 +9813,7 @@
       </c>
       <c r="C552" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9949,7 +9949,7 @@
       </c>
       <c r="C560" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9983,7 +9983,7 @@
       </c>
       <c r="C562" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10034,7 +10034,7 @@
       </c>
       <c r="C565" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10051,7 +10051,7 @@
       </c>
       <c r="C566" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10068,7 +10068,7 @@
       </c>
       <c r="C567" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10170,7 +10170,7 @@
       </c>
       <c r="C573" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10357,7 +10357,7 @@
       </c>
       <c r="C584" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10663,7 +10663,7 @@
       </c>
       <c r="C602" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -10748,7 +10748,7 @@
       </c>
       <c r="C607" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10816,7 +10816,7 @@
       </c>
       <c r="C611" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10918,7 +10918,7 @@
       </c>
       <c r="C617" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11071,7 +11071,7 @@
       </c>
       <c r="C626" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11258,7 +11258,7 @@
       </c>
       <c r="C637" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11360,7 +11360,7 @@
       </c>
       <c r="C643" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11377,7 +11377,7 @@
       </c>
       <c r="C644" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11394,7 +11394,7 @@
       </c>
       <c r="C645" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11411,7 +11411,7 @@
       </c>
       <c r="C646" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11428,7 +11428,7 @@
       </c>
       <c r="C647" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11462,7 +11462,7 @@
       </c>
       <c r="C649" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11615,7 +11615,7 @@
       </c>
       <c r="C658" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11751,7 +11751,7 @@
       </c>
       <c r="C666" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11819,7 +11819,7 @@
       </c>
       <c r="C670" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11853,7 +11853,7 @@
       </c>
       <c r="C672" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11870,7 +11870,7 @@
       </c>
       <c r="C673" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11904,7 +11904,7 @@
       </c>
       <c r="C675" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11938,7 +11938,7 @@
       </c>
       <c r="C677" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11972,7 +11972,7 @@
       </c>
       <c r="C679" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12006,7 +12006,7 @@
       </c>
       <c r="C681" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12074,7 +12074,7 @@
       </c>
       <c r="C685" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12125,7 +12125,7 @@
       </c>
       <c r="C688" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12210,7 +12210,7 @@
       </c>
       <c r="C693" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12227,7 +12227,7 @@
       </c>
       <c r="C694" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12244,7 +12244,7 @@
       </c>
       <c r="C695" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12278,7 +12278,7 @@
       </c>
       <c r="C697" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12295,7 +12295,7 @@
       </c>
       <c r="C698" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12312,7 +12312,7 @@
       </c>
       <c r="C699" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12363,7 +12363,7 @@
       </c>
       <c r="C702" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12397,7 +12397,7 @@
       </c>
       <c r="C704" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12448,7 +12448,7 @@
       </c>
       <c r="C707" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12465,7 +12465,7 @@
       </c>
       <c r="C708" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12601,7 +12601,7 @@
       </c>
       <c r="C716" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12618,7 +12618,7 @@
       </c>
       <c r="C717" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12652,7 +12652,7 @@
       </c>
       <c r="C719" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12907,7 +12907,7 @@
       </c>
       <c r="C734" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13179,7 +13179,7 @@
       </c>
       <c r="C750" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -13196,7 +13196,7 @@
       </c>
       <c r="C751" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13213,7 +13213,7 @@
       </c>
       <c r="C752" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13230,7 +13230,7 @@
       </c>
       <c r="C753" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13349,7 +13349,7 @@
       </c>
       <c r="C760" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13417,7 +13417,7 @@
       </c>
       <c r="C764" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13519,7 +13519,7 @@
       </c>
       <c r="C770" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13553,7 +13553,7 @@
       </c>
       <c r="C772" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -13621,7 +13621,7 @@
       </c>
       <c r="C776" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13706,7 +13706,7 @@
       </c>
       <c r="C781" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13723,7 +13723,7 @@
       </c>
       <c r="C782" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -13808,7 +13808,7 @@
       </c>
       <c r="C787" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13961,7 +13961,7 @@
       </c>
       <c r="C796" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14114,7 +14114,7 @@
       </c>
       <c r="C805" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14148,7 +14148,7 @@
       </c>
       <c r="C807" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -14216,7 +14216,7 @@
       </c>
       <c r="C811" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14335,7 +14335,7 @@
       </c>
       <c r="C818" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14352,7 +14352,7 @@
       </c>
       <c r="C819" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -14505,7 +14505,7 @@
       </c>
       <c r="C828" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14522,7 +14522,7 @@
       </c>
       <c r="C829" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14641,7 +14641,7 @@
       </c>
       <c r="C836" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14675,7 +14675,7 @@
       </c>
       <c r="C838" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14692,7 +14692,7 @@
       </c>
       <c r="C839" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14709,7 +14709,7 @@
       </c>
       <c r="C840" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14743,7 +14743,7 @@
       </c>
       <c r="C842" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14777,7 +14777,7 @@
       </c>
       <c r="C844" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14828,7 +14828,7 @@
       </c>
       <c r="C847" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14845,7 +14845,7 @@
       </c>
       <c r="C848" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -15083,7 +15083,7 @@
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15134,7 +15134,7 @@
       </c>
       <c r="C865" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15168,7 +15168,7 @@
       </c>
       <c r="C867" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15253,7 +15253,7 @@
       </c>
       <c r="C872" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15270,7 +15270,7 @@
       </c>
       <c r="C873" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15304,7 +15304,7 @@
       </c>
       <c r="C875" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15491,7 +15491,7 @@
       </c>
       <c r="C886" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15508,7 +15508,7 @@
       </c>
       <c r="C887" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15576,7 +15576,7 @@
       </c>
       <c r="C891" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15593,7 +15593,7 @@
       </c>
       <c r="C892" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15678,7 +15678,7 @@
       </c>
       <c r="C897" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15712,7 +15712,7 @@
       </c>
       <c r="C899" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15729,7 +15729,7 @@
       </c>
       <c r="C900" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15797,7 +15797,7 @@
       </c>
       <c r="C904" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15831,7 +15831,7 @@
       </c>
       <c r="C906" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15865,7 +15865,7 @@
       </c>
       <c r="C908" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15916,7 +15916,7 @@
       </c>
       <c r="C911" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16120,7 +16120,7 @@
       </c>
       <c r="C923" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16171,7 +16171,7 @@
       </c>
       <c r="C926" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16188,7 +16188,7 @@
       </c>
       <c r="C927" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16273,7 +16273,7 @@
       </c>
       <c r="C932" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16290,7 +16290,7 @@
       </c>
       <c r="C933" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16358,7 +16358,7 @@
       </c>
       <c r="C937" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16375,7 +16375,7 @@
       </c>
       <c r="C938" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16528,7 +16528,7 @@
       </c>
       <c r="C947" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16579,7 +16579,7 @@
       </c>
       <c r="C950" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16630,7 +16630,7 @@
       </c>
       <c r="C953" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16698,7 +16698,7 @@
       </c>
       <c r="C957" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16715,7 +16715,7 @@
       </c>
       <c r="C958" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16732,7 +16732,7 @@
       </c>
       <c r="C959" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16817,7 +16817,7 @@
       </c>
       <c r="C964" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16885,7 +16885,7 @@
       </c>
       <c r="C968" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16902,7 +16902,7 @@
       </c>
       <c r="C969" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16987,7 +16987,7 @@
       </c>
       <c r="C974" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17021,7 +17021,7 @@
       </c>
       <c r="C976" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17174,7 +17174,7 @@
       </c>
       <c r="C985" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17276,7 +17276,7 @@
       </c>
       <c r="C991" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17310,7 +17310,7 @@
       </c>
       <c r="C993" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17412,7 +17412,7 @@
       </c>
       <c r="C999" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17463,7 +17463,7 @@
       </c>
       <c r="C1002" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17565,7 +17565,7 @@
       </c>
       <c r="C1008" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17633,7 +17633,7 @@
       </c>
       <c r="C1012" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17735,7 +17735,7 @@
       </c>
       <c r="C1018" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17752,7 +17752,7 @@
       </c>
       <c r="C1019" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17769,7 +17769,7 @@
       </c>
       <c r="C1020" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17786,7 +17786,7 @@
       </c>
       <c r="C1021" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17820,7 +17820,7 @@
       </c>
       <c r="C1023" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17922,7 +17922,7 @@
       </c>
       <c r="C1029" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -17990,7 +17990,7 @@
       </c>
       <c r="C1033" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -18007,7 +18007,7 @@
       </c>
       <c r="C1034" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18024,7 +18024,7 @@
       </c>
       <c r="C1035" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18041,7 +18041,7 @@
       </c>
       <c r="C1036" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18279,7 +18279,7 @@
       </c>
       <c r="C1050" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18330,7 +18330,7 @@
       </c>
       <c r="C1053" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18534,7 +18534,7 @@
       </c>
       <c r="C1065" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18585,7 +18585,7 @@
       </c>
       <c r="C1068" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18653,7 +18653,7 @@
       </c>
       <c r="C1072" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18687,7 +18687,7 @@
       </c>
       <c r="C1074" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18738,7 +18738,7 @@
       </c>
       <c r="C1077" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18806,7 +18806,7 @@
       </c>
       <c r="C1081" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18908,7 +18908,7 @@
       </c>
       <c r="C1087" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18959,7 +18959,7 @@
       </c>
       <c r="C1090" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19027,7 +19027,7 @@
       </c>
       <c r="C1094" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19163,7 +19163,7 @@
       </c>
       <c r="C1102" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19197,7 +19197,7 @@
       </c>
       <c r="C1104" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19265,7 +19265,7 @@
       </c>
       <c r="C1108" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19282,7 +19282,7 @@
       </c>
       <c r="C1109" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19316,7 +19316,7 @@
       </c>
       <c r="C1111" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19401,7 +19401,7 @@
       </c>
       <c r="C1116" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19469,7 +19469,7 @@
       </c>
       <c r="C1120" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19486,7 +19486,7 @@
       </c>
       <c r="C1121" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19554,7 +19554,7 @@
       </c>
       <c r="C1125" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19588,7 +19588,7 @@
       </c>
       <c r="C1127" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19656,7 +19656,7 @@
       </c>
       <c r="C1131" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19690,7 +19690,7 @@
       </c>
       <c r="C1133" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19724,7 +19724,7 @@
       </c>
       <c r="C1135" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19877,7 +19877,7 @@
       </c>
       <c r="C1144" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19945,7 +19945,7 @@
       </c>
       <c r="C1148" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19962,7 +19962,7 @@
       </c>
       <c r="C1149" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20013,7 +20013,7 @@
       </c>
       <c r="C1152" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20115,7 +20115,7 @@
       </c>
       <c r="C1158" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20268,7 +20268,7 @@
       </c>
       <c r="C1167" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20336,7 +20336,7 @@
       </c>
       <c r="C1171" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20387,7 +20387,7 @@
       </c>
       <c r="C1174" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20404,7 +20404,7 @@
       </c>
       <c r="C1175" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20744,7 +20744,7 @@
       </c>
       <c r="C1195" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20829,7 +20829,7 @@
       </c>
       <c r="C1200" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -20863,7 +20863,7 @@
       </c>
       <c r="C1202" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20897,7 +20897,7 @@
       </c>
       <c r="C1204" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20931,7 +20931,7 @@
       </c>
       <c r="C1206" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20999,7 +20999,7 @@
       </c>
       <c r="C1210" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21016,7 +21016,7 @@
       </c>
       <c r="C1211" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21033,7 +21033,7 @@
       </c>
       <c r="C1212" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21050,7 +21050,7 @@
       </c>
       <c r="C1213" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21084,7 +21084,7 @@
       </c>
       <c r="C1215" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21152,7 +21152,7 @@
       </c>
       <c r="C1219" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21169,7 +21169,7 @@
       </c>
       <c r="C1220" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21186,7 +21186,7 @@
       </c>
       <c r="C1221" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21220,7 +21220,7 @@
       </c>
       <c r="C1223" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21237,7 +21237,7 @@
       </c>
       <c r="C1224" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21305,7 +21305,7 @@
       </c>
       <c r="C1228" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -21322,7 +21322,7 @@
       </c>
       <c r="C1229" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21339,7 +21339,7 @@
       </c>
       <c r="C1230" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21356,7 +21356,7 @@
       </c>
       <c r="C1231" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21373,7 +21373,7 @@
       </c>
       <c r="C1232" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21390,7 +21390,7 @@
       </c>
       <c r="C1233" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21441,7 +21441,7 @@
       </c>
       <c r="C1236" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21543,7 +21543,7 @@
       </c>
       <c r="C1242" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21577,7 +21577,7 @@
       </c>
       <c r="C1244" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21747,7 +21747,7 @@
       </c>
       <c r="C1254" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21883,7 +21883,7 @@
       </c>
       <c r="C1262" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22002,7 +22002,7 @@
       </c>
       <c r="C1269" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22036,7 +22036,7 @@
       </c>
       <c r="C1271" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22053,7 +22053,7 @@
       </c>
       <c r="C1272" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22189,7 +22189,7 @@
       </c>
       <c r="C1280" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -22274,7 +22274,7 @@
       </c>
       <c r="C1285" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22325,7 +22325,7 @@
       </c>
       <c r="C1288" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22376,7 +22376,7 @@
       </c>
       <c r="C1291" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22410,7 +22410,7 @@
       </c>
       <c r="C1293" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22427,7 +22427,7 @@
       </c>
       <c r="C1294" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22512,7 +22512,7 @@
       </c>
       <c r="C1299" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22563,7 +22563,7 @@
       </c>
       <c r="C1302" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22614,7 +22614,7 @@
       </c>
       <c r="C1305" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22631,7 +22631,7 @@
       </c>
       <c r="C1306" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22750,7 +22750,7 @@
       </c>
       <c r="C1313" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22784,7 +22784,7 @@
       </c>
       <c r="C1315" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22801,7 +22801,7 @@
       </c>
       <c r="C1316" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22852,7 +22852,7 @@
       </c>
       <c r="C1319" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22903,7 +22903,7 @@
       </c>
       <c r="C1322" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22971,7 +22971,7 @@
       </c>
       <c r="C1326" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -22988,7 +22988,7 @@
       </c>
       <c r="C1327" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23005,7 +23005,7 @@
       </c>
       <c r="C1328" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23022,7 +23022,7 @@
       </c>
       <c r="C1329" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23090,7 +23090,7 @@
       </c>
       <c r="C1333" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23226,7 +23226,7 @@
       </c>
       <c r="C1341" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23260,7 +23260,7 @@
       </c>
       <c r="C1343" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23294,7 +23294,7 @@
       </c>
       <c r="C1345" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23447,7 +23447,7 @@
       </c>
       <c r="C1354" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23498,7 +23498,7 @@
       </c>
       <c r="C1357" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23617,7 +23617,7 @@
       </c>
       <c r="C1364" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23634,7 +23634,7 @@
       </c>
       <c r="C1365" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23753,7 +23753,7 @@
       </c>
       <c r="C1372" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23787,7 +23787,7 @@
       </c>
       <c r="C1374" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23855,7 +23855,7 @@
       </c>
       <c r="C1378" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23889,7 +23889,7 @@
       </c>
       <c r="C1380" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23906,7 +23906,7 @@
       </c>
       <c r="C1381" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23940,7 +23940,7 @@
       </c>
       <c r="C1383" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23957,7 +23957,7 @@
       </c>
       <c r="C1384" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24042,7 +24042,7 @@
       </c>
       <c r="C1389" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24161,7 +24161,7 @@
       </c>
       <c r="C1396" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24246,7 +24246,7 @@
       </c>
       <c r="C1401" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24263,7 +24263,7 @@
       </c>
       <c r="C1402" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24297,7 +24297,7 @@
       </c>
       <c r="C1404" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24331,7 +24331,7 @@
       </c>
       <c r="C1406" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24365,7 +24365,7 @@
       </c>
       <c r="C1408" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>

</xml_diff>